<commit_message>
Added Comptroller source object profile
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_SM_FOU_NacuboSourceProfile_Regression_001.xlsx
+++ b/src/main/java/TestSuite/MDOT/Scenarios/MDOT/TS_SM_FOU_NacuboSourceProfile_Regression_001.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\MDOT\Scenarios\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{744F4450-BCCE-4A0C-90C0-F9CBBF4FA999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC80C6F1-4EE2-44DB-A992-9355A940F338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{75A34C94-B21C-4705-BA56-409F86A5FE33}"/>
+    <workbookView xWindow="420" yWindow="890" windowWidth="18780" windowHeight="9910" xr2:uid="{75A34C94-B21C-4705-BA56-409F86A5FE33}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="35">
   <si>
     <t>BusinessModule</t>
   </si>
@@ -133,6 +133,12 @@
   </si>
   <si>
     <t>Confirm Alert Box</t>
+  </si>
+  <si>
+    <t>Login_Logout</t>
+  </si>
+  <si>
+    <t>Logout</t>
   </si>
 </sst>
 </file>
@@ -529,10 +535,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A358F6FE-A098-4E91-81D3-17486A39482C}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="22" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -865,6 +871,26 @@
         <v>1</v>
       </c>
     </row>
+    <row r="17" spans="1:6" ht="22" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="2">
+        <v>1</v>
+      </c>
+      <c r="F17" s="2">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>